<commit_message>
Added homework to algorithm complexity lection
</commit_message>
<xml_diff>
--- a/homework/09.alorithms-and-data-structures/09.alorithms-and-data-structures.xlsx
+++ b/homework/09.alorithms-and-data-structures/09.alorithms-and-data-structures.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\java-course\java-course\homework\09.alorithms-and-data-structures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bilyukov\courses\java\java-course\homework\09.alorithms-and-data-structures\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,12 +24,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Задача</t>
   </si>
   <si>
     <t>Информация</t>
+  </si>
+  <si>
+    <t>Направете проучване и имплементирайте алгоритъма Bucket Sort</t>
+  </si>
+  <si>
+    <t>Направете проучване и имплементирайте алгоритъма Quick Sort</t>
+  </si>
+  <si>
+    <t>Направете програма, която приема изречение и подрежда по азбучен ред всички думи от него</t>
+  </si>
+  <si>
+    <t>Направете програма, която приема 10 числа. Подредете във възходящ ред всички четни числа в масив. Подредете всички нечетни числа в нискодящ ред в друг масив</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Направете програма, която приема 30 числа и намира всички тройки еднакви числа </t>
   </si>
 </sst>
 </file>
@@ -371,7 +386,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,24 +403,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>